<commit_message>
new DB. Fix check profile and add_subject on name and hours
</commit_message>
<xml_diff>
--- a/generated/Таблица_распределения_09.25.20.xlsx
+++ b/generated/Таблица_распределения_09.25.20.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>ФИО</t>
   </si>
@@ -29,157 +29,115 @@
     <t>Часы</t>
   </si>
   <si>
+    <t>Галлиулина Эльвира Сайфуловна</t>
+  </si>
+  <si>
+    <t>История</t>
+  </si>
+  <si>
+    <t>3020в</t>
+  </si>
+  <si>
+    <t>3021в</t>
+  </si>
+  <si>
+    <t>Основы философии</t>
+  </si>
+  <si>
+    <t>3920в</t>
+  </si>
+  <si>
+    <t>3921в</t>
+  </si>
+  <si>
+    <t>Философия</t>
+  </si>
+  <si>
+    <t>Итого:</t>
+  </si>
+  <si>
+    <t>Погудина Лада геннадьевна</t>
+  </si>
+  <si>
+    <t>Математика</t>
+  </si>
+  <si>
+    <t>Элементы высшей математики</t>
+  </si>
+  <si>
+    <t>Дискретная математика</t>
+  </si>
+  <si>
+    <t>Теория вероятностей и математическая статистика</t>
+  </si>
+  <si>
+    <t>Кабанова Людмила Геннадьевна</t>
+  </si>
+  <si>
+    <t>Родная литература</t>
+  </si>
+  <si>
+    <t>Литература</t>
+  </si>
+  <si>
+    <t>Русский язык</t>
+  </si>
+  <si>
+    <t>Русский язык и культура речи</t>
+  </si>
+  <si>
+    <t>Соларёва Юлия Сергеевна</t>
+  </si>
+  <si>
+    <t>Экономика</t>
+  </si>
+  <si>
+    <t>Право</t>
+  </si>
+  <si>
+    <t>Основы экономической теории</t>
+  </si>
+  <si>
+    <t>Экономика организации</t>
+  </si>
+  <si>
+    <t>Международные расчёты по экспортно-импортным операциям</t>
+  </si>
+  <si>
+    <t>Выполнение работ по профессии "Агент банка"</t>
+  </si>
+  <si>
     <t>Сидорова Светлана Витальевна</t>
   </si>
   <si>
-    <t>Иностранный язык 117ч</t>
-  </si>
-  <si>
-    <t>3020в</t>
-  </si>
-  <si>
-    <t>3021в</t>
-  </si>
-  <si>
-    <t>ИЯ в ПД 68ч</t>
-  </si>
-  <si>
-    <t>3920в</t>
-  </si>
-  <si>
-    <t>ИЯ в ПД 72ч</t>
-  </si>
-  <si>
-    <t>3921в</t>
-  </si>
-  <si>
-    <t>ИЯ в ПД 74ч</t>
-  </si>
-  <si>
-    <t>Итого:</t>
-  </si>
-  <si>
-    <t>Кабанова Людмила Геннадьевна</t>
-  </si>
-  <si>
-    <t>Литература 73ч</t>
-  </si>
-  <si>
-    <t>Русский язык 78ч</t>
-  </si>
-  <si>
-    <t>Родная литература 44ч</t>
-  </si>
-  <si>
-    <t>Русский язык и культура речи 68ч</t>
-  </si>
-  <si>
-    <t>Русский язык и культура речи 72ч</t>
-  </si>
-  <si>
-    <t>Русский язык и культура речи 48ч</t>
+    <t>Иностранный язык</t>
+  </si>
+  <si>
+    <t>ИЯ в ПД</t>
   </si>
   <si>
     <t>Мелешкин Илья Петрович</t>
   </si>
   <si>
-    <t>Физическая культура 117ч</t>
-  </si>
-  <si>
-    <t>Физическая культура 68ч</t>
-  </si>
-  <si>
-    <t>Адаптивная физическая культура 72ч</t>
-  </si>
-  <si>
-    <t>Физическая культура 74ч</t>
-  </si>
-  <si>
-    <t>Соларёва Юлия Сергеевна</t>
-  </si>
-  <si>
-    <t>Экономика 200ч</t>
-  </si>
-  <si>
-    <t>Право 162ч</t>
-  </si>
-  <si>
-    <t>Экономика организации 85ч</t>
-  </si>
-  <si>
-    <t>Бухгалтерский учёт 48ч</t>
-  </si>
-  <si>
-    <t>Выполнение работ по профессии "Агент банка" 228ч</t>
-  </si>
-  <si>
-    <t>Организация безналичных расчётов 40ч</t>
-  </si>
-  <si>
-    <t>Экономика организации 72ч</t>
-  </si>
-  <si>
-    <t>Кассовые операции банков 156ч</t>
-  </si>
-  <si>
-    <t>Организация бухгалтерского учёта в банках 40ч</t>
-  </si>
-  <si>
-    <t>Международные расчёты по экспортно-импортным операциям 60ч</t>
-  </si>
-  <si>
-    <t>Галлиулина Эльвира Сайфуловна</t>
-  </si>
-  <si>
-    <t>История 117ч</t>
-  </si>
-  <si>
-    <t>История 48ч</t>
-  </si>
-  <si>
-    <t>Основы философии 34ч</t>
-  </si>
-  <si>
-    <t>История 51ч</t>
-  </si>
-  <si>
-    <t>Философия 40ч</t>
-  </si>
-  <si>
-    <t>Погудина Лада геннадьевна</t>
-  </si>
-  <si>
-    <t>Математика 234ч</t>
-  </si>
-  <si>
-    <t>Математика 51ч</t>
-  </si>
-  <si>
-    <t>Элементы высшей математики 48ч</t>
-  </si>
-  <si>
-    <t>Элементы высшей математики 80ч</t>
-  </si>
-  <si>
-    <t>Дискретная математика 42ч</t>
-  </si>
-  <si>
-    <t>Теория вероятностей и математическая статистика 42ч</t>
+    <t>Физическая культура</t>
+  </si>
+  <si>
+    <t>Адаптивная физическая культура</t>
   </si>
   <si>
     <t>Овчинников Антон Викторович</t>
   </si>
   <si>
-    <t>Основы проектирования БД 64ч</t>
-  </si>
-  <si>
-    <t>Инженерная компьютерная графика 64ч</t>
-  </si>
-  <si>
-    <t>Проектирование и дизайн информационных систем 226ч</t>
-  </si>
-  <si>
-    <t>Разработка кода информационных систем 192ч</t>
+    <t>Основы проектирования БД</t>
+  </si>
+  <si>
+    <t>Инженерная компьютерная графика</t>
+  </si>
+  <si>
+    <t>Проектирование и дизайн информационных систем</t>
+  </si>
+  <si>
+    <t>Разработка кода информационных систем</t>
   </si>
 </sst>
 </file>
@@ -518,7 +476,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,215 +577,215 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
+      <c r="C8">
+        <v>3907</v>
       </c>
       <c r="D8">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3907</v>
       </c>
       <c r="D9">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>3939</v>
+        <v>3918</v>
       </c>
       <c r="D10">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" t="s">
-        <v>13</v>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3918</v>
       </c>
       <c r="D11">
-        <v>916</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12"/>
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>3007</v>
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>73</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>3007</v>
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>3007</v>
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>3018</v>
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>73</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>3018</v>
+        <v>3939</v>
       </c>
       <c r="D16">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17"/>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>3018</v>
+      <c r="B17"/>
+      <c r="C17" t="s">
+        <v>12</v>
       </c>
       <c r="D17">
-        <v>44</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18"/>
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>3019</v>
+        <v>3007</v>
       </c>
       <c r="D18">
-        <v>73</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19"/>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="D19">
-        <v>78</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>3019</v>
       </c>
       <c r="D20">
-        <v>44</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>73</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>78</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>3039</v>
       </c>
       <c r="D23">
-        <v>44</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>3907</v>
       </c>
       <c r="D24">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -836,70 +794,70 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>3039</v>
+        <v>3939</v>
       </c>
       <c r="D27">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>3039</v>
+        <v>3939</v>
       </c>
       <c r="D28">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>3039</v>
+        <v>3939</v>
       </c>
       <c r="D29">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30"/>
-      <c r="B30" t="s">
+      <c r="B30"/>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31"/>
       <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C31" t="s">
-        <v>11</v>
+      <c r="C31">
+        <v>3007</v>
       </c>
       <c r="D31">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -908,679 +866,775 @@
         <v>20</v>
       </c>
       <c r="C32">
-        <v>3939</v>
+        <v>3007</v>
       </c>
       <c r="D32">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33" t="s">
-        <v>13</v>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>3007</v>
       </c>
       <c r="D33">
-        <v>1358</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
+      <c r="A34"/>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>3007</v>
+        <v>3018</v>
       </c>
       <c r="D34">
-        <v>117</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C35">
         <v>3018</v>
       </c>
       <c r="D35">
-        <v>117</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="D36">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>3019</v>
       </c>
       <c r="D37">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="C38">
+        <v>3019</v>
       </c>
       <c r="D38">
-        <v>117</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C39">
-        <v>3039</v>
+        <v>3019</v>
       </c>
       <c r="D39">
-        <v>117</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D40">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42">
-        <v>3939</v>
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
       </c>
       <c r="D42">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43"/>
-      <c r="B43"/>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>916</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>26</v>
-      </c>
+      <c r="A44"/>
       <c r="B44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44">
-        <v>3007</v>
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
       </c>
       <c r="D44">
-        <v>200</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45">
-        <v>3007</v>
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>162</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>3039</v>
       </c>
       <c r="D46">
-        <v>200</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>3039</v>
       </c>
       <c r="D47">
-        <v>162</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="C48">
+        <v>3039</v>
       </c>
       <c r="D48">
-        <v>200</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C49">
+        <v>3907</v>
       </c>
       <c r="D49">
-        <v>162</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="C50">
+        <v>3918</v>
       </c>
       <c r="D50">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D51">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52">
-        <v>228</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>3939</v>
       </c>
       <c r="D53">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54"/>
-      <c r="B54" t="s">
-        <v>33</v>
-      </c>
+      <c r="B54"/>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D54">
-        <v>72</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55"/>
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
       <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="C55">
+        <v>3007</v>
       </c>
       <c r="D55">
-        <v>156</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>3007</v>
       </c>
       <c r="D56">
-        <v>40</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D57">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58"/>
-      <c r="B58"/>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D58">
-        <v>1815</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>37</v>
-      </c>
+      <c r="A59"/>
       <c r="B59" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59">
-        <v>3007</v>
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
       </c>
       <c r="D59">
-        <v>117</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60">
-        <v>3018</v>
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
       </c>
       <c r="D60">
-        <v>117</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C61">
-        <v>3019</v>
+        <v>3918</v>
       </c>
       <c r="D61">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="C62">
+        <v>3918</v>
       </c>
       <c r="D62">
-        <v>117</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D63">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64">
-        <v>3039</v>
+        <v>27</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
       </c>
       <c r="D64">
-        <v>117</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65">
-        <v>3918</v>
+        <v>28</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
       </c>
       <c r="D65">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66">
-        <v>34</v>
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67"/>
-      <c r="B67" t="s">
-        <v>41</v>
-      </c>
+      <c r="B67"/>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D67">
-        <v>51</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68"/>
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
       <c r="B68" t="s">
-        <v>39</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="C68">
+        <v>3007</v>
       </c>
       <c r="D68">
-        <v>48</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C69" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="C69">
+        <v>3018</v>
       </c>
       <c r="D69">
-        <v>40</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C70">
-        <v>3939</v>
+        <v>3019</v>
       </c>
       <c r="D70">
-        <v>48</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71"/>
-      <c r="B71"/>
+      <c r="B71" t="s">
+        <v>31</v>
+      </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D71">
-        <v>971</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>43</v>
-      </c>
+      <c r="A72"/>
       <c r="B72" t="s">
-        <v>44</v>
-      </c>
-      <c r="C72">
-        <v>3007</v>
+        <v>31</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
       </c>
       <c r="D72">
-        <v>234</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C73">
-        <v>3018</v>
+        <v>3039</v>
       </c>
       <c r="D73">
-        <v>234</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C74">
-        <v>3019</v>
+        <v>3907</v>
       </c>
       <c r="D74">
-        <v>234</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>44</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="C75">
+        <v>3918</v>
       </c>
       <c r="D75">
-        <v>234</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C76" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D76">
-        <v>234</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>44</v>
-      </c>
-      <c r="C77">
-        <v>3039</v>
+        <v>32</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
       </c>
       <c r="D77">
-        <v>234</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>45</v>
-      </c>
-      <c r="C78" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="C78">
+        <v>3939</v>
       </c>
       <c r="D78">
-        <v>51</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79"/>
-      <c r="B79" t="s">
-        <v>46</v>
-      </c>
+      <c r="B79"/>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D79">
-        <v>48</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80"/>
+      <c r="A80" t="s">
+        <v>33</v>
+      </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C80">
-        <v>3939</v>
+        <v>3007</v>
       </c>
       <c r="D80">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C81">
-        <v>3939</v>
+        <v>3018</v>
       </c>
       <c r="D81">
-        <v>42</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C82">
-        <v>3939</v>
+        <v>3019</v>
       </c>
       <c r="D82">
-        <v>42</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83"/>
-      <c r="B83"/>
+      <c r="B83" t="s">
+        <v>34</v>
+      </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D83">
-        <v>1667</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" t="s">
-        <v>50</v>
-      </c>
+      <c r="A84"/>
       <c r="B84" t="s">
-        <v>51</v>
-      </c>
-      <c r="C84">
-        <v>3939</v>
+        <v>34</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
       </c>
       <c r="D84">
-        <v>64</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C85">
-        <v>3939</v>
+        <v>3039</v>
       </c>
       <c r="D85">
-        <v>64</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C86">
-        <v>3939</v>
+        <v>3907</v>
       </c>
       <c r="D86">
-        <v>226</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C87">
-        <v>3939</v>
+        <v>3918</v>
       </c>
       <c r="D87">
-        <v>192</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88"/>
-      <c r="B88"/>
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D88">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89"/>
+      <c r="B89" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90"/>
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90">
+        <v>3939</v>
+      </c>
+      <c r="D90">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92">
+        <v>3939</v>
+      </c>
+      <c r="D92">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93"/>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93">
+        <v>3939</v>
+      </c>
+      <c r="D93">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94"/>
+      <c r="B94" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94">
+        <v>3939</v>
+      </c>
+      <c r="D94">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95"/>
+      <c r="B95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95">
+        <v>3939</v>
+      </c>
+      <c r="D95">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96">
         <v>546</v>
       </c>
     </row>

</xml_diff>